<commit_message>
added holidays and exams (Aug)
</commit_message>
<xml_diff>
--- a/data/excel_files/FormattedAug2023.xlsx
+++ b/data/excel_files/FormattedAug2023.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -31,10 +31,25 @@
     <t>Holiday</t>
   </si>
   <si>
-    <t>MenuItem</t>
+    <t>CouponMand</t>
+  </si>
+  <si>
+    <t>Exam</t>
+  </si>
+  <si>
+    <t>Coupon15</t>
+  </si>
+  <si>
+    <t>Coupon25</t>
+  </si>
+  <si>
+    <t>Coupon30</t>
   </si>
   <si>
     <t>BreakFast</t>
+  </si>
+  <si>
+    <t>Acad</t>
   </si>
   <si>
     <t>Lunch</t>
@@ -84,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -93,6 +108,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -336,74 +354,134 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>45139.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5">
         <v>90.0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>23.0</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45139</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5">
         <v>126.0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>71.0</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45139</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="4">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="5">
         <v>26.0</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45139</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5">
         <v>63.0</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45140</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <v>52.0</v>
@@ -411,14 +489,26 @@
       <c r="D6" s="1">
         <v>79.0</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45140</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>76.0</v>
@@ -426,14 +516,26 @@
       <c r="D7" s="1">
         <v>115.0</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45140</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1">
         <v>4.0</v>
@@ -441,14 +543,26 @@
       <c r="D8" s="1">
         <v>43.0</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45140</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <v>137.0</v>
@@ -456,14 +570,26 @@
       <c r="D9" s="1">
         <v>161.0</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45141</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>83.0</v>
@@ -471,14 +597,26 @@
       <c r="D10" s="1">
         <v>116.0</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="5">
+      <c r="A11" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45141</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>177.0</v>
@@ -486,14 +624,26 @@
       <c r="D11" s="1">
         <v>150.0</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="5">
+      <c r="A12" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45141</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
         <v>0.0</v>
@@ -501,14 +651,26 @@
       <c r="D12" s="1">
         <v>56.0</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="5">
+      <c r="A13" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45141</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
         <v>66.0</v>
@@ -516,14 +678,26 @@
       <c r="D13" s="1">
         <v>128.0</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="5">
+      <c r="A14" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45142</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>76.0</v>
@@ -531,26 +705,50 @@
       <c r="D14" s="1">
         <v>143.0</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="5">
+      <c r="A15" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45142</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>128.0</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="5">
+      <c r="A16" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45142</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>3.0</v>
@@ -558,14 +756,26 @@
       <c r="D16" s="1">
         <v>80.0</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="5">
+      <c r="A17" s="6">
         <f>A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45142</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>55.0</v>
@@ -573,14 +783,26 @@
       <c r="D17" s="1">
         <v>156.0</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="5">
+      <c r="A18" s="6">
         <f t="shared" ref="A18:A21" si="1">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45143</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1">
         <v>42.0</v>
@@ -588,14 +810,26 @@
       <c r="D18" s="1">
         <v>116.0</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="5">
+      <c r="A19" s="6">
         <f t="shared" si="1"/>
         <v>45143</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1">
         <v>152.0</v>
@@ -603,14 +837,26 @@
       <c r="D19" s="1">
         <v>184.0</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="5">
+      <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>45143</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1">
         <v>5.0</v>
@@ -618,14 +864,26 @@
       <c r="D20" s="1">
         <v>64.0</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="5">
+      <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>45143</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1">
         <v>24.0</v>
@@ -633,14 +891,26 @@
       <c r="D21" s="1">
         <v>106.0</v>
       </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="5">
+      <c r="A22" s="6">
         <f t="shared" ref="A22:A25" si="2">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45144</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1">
         <v>35.0</v>
@@ -648,14 +918,26 @@
       <c r="D22" s="1">
         <v>127.0</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="5">
+      <c r="A23" s="6">
         <f t="shared" si="2"/>
         <v>45144</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
         <v>87.0</v>
@@ -663,14 +945,26 @@
       <c r="D23" s="1">
         <v>138.0</v>
       </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="5">
+      <c r="A24" s="6">
         <f t="shared" si="2"/>
         <v>45144</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1">
         <v>4.0</v>
@@ -678,14 +972,26 @@
       <c r="D24" s="1">
         <v>100.0</v>
       </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="5">
+      <c r="A25" s="6">
         <f t="shared" si="2"/>
         <v>45144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
         <v>93.0</v>
@@ -693,14 +999,26 @@
       <c r="D25" s="1">
         <v>245.0</v>
       </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="5">
+      <c r="A26" s="6">
         <f t="shared" ref="A26:A29" si="3">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45145</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1">
         <v>37.0</v>
@@ -708,14 +1026,26 @@
       <c r="D26" s="1">
         <v>211.0</v>
       </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="5">
+      <c r="A27" s="6">
         <f t="shared" si="3"/>
         <v>45145</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C27" s="1">
         <v>124.0</v>
@@ -723,14 +1053,26 @@
       <c r="D27" s="1">
         <v>274.0</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="5">
+      <c r="A28" s="6">
         <f t="shared" si="3"/>
         <v>45145</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1">
         <v>10.0</v>
@@ -738,14 +1080,26 @@
       <c r="D28" s="1">
         <v>173.0</v>
       </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="5">
+      <c r="A29" s="6">
         <f t="shared" si="3"/>
         <v>45145</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1">
         <v>36.0</v>
@@ -753,14 +1107,26 @@
       <c r="D29" s="1">
         <v>295.0</v>
       </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="5">
+      <c r="A30" s="6">
         <f t="shared" ref="A30:A33" si="4">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45146</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1">
         <v>35.0</v>
@@ -768,14 +1134,26 @@
       <c r="D30" s="1">
         <v>274.0</v>
       </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="5">
+      <c r="A31" s="6">
         <f t="shared" si="4"/>
         <v>45146</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C31" s="1">
         <v>123.0</v>
@@ -783,14 +1161,26 @@
       <c r="D31" s="1">
         <v>373.0</v>
       </c>
+      <c r="E31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="5">
+      <c r="A32" s="6">
         <f t="shared" si="4"/>
         <v>45146</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C32" s="1">
         <v>10.0</v>
@@ -798,14 +1188,26 @@
       <c r="D32" s="1">
         <v>221.0</v>
       </c>
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="5">
+      <c r="A33" s="6">
         <f t="shared" si="4"/>
         <v>45146</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C33" s="1">
         <v>53.0</v>
@@ -813,14 +1215,26 @@
       <c r="D33" s="1">
         <v>297.0</v>
       </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="5">
+      <c r="A34" s="6">
         <f t="shared" ref="A34:A37" si="5">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45147</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1">
         <v>27.0</v>
@@ -828,14 +1242,26 @@
       <c r="D34" s="1">
         <v>306.0</v>
       </c>
+      <c r="E34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="5">
+      <c r="A35" s="6">
         <f t="shared" si="5"/>
         <v>45147</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C35" s="1">
         <v>107.0</v>
@@ -843,14 +1269,26 @@
       <c r="D35" s="1">
         <v>367.0</v>
       </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="5">
+      <c r="A36" s="6">
         <f t="shared" si="5"/>
         <v>45147</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C36" s="1">
         <v>3.0</v>
@@ -858,14 +1296,26 @@
       <c r="D36" s="1">
         <v>169.0</v>
       </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="5">
+      <c r="A37" s="6">
         <f t="shared" si="5"/>
         <v>45147</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C37" s="1">
         <v>58.0</v>
@@ -873,14 +1323,26 @@
       <c r="D37" s="1">
         <v>430.0</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="5">
+      <c r="A38" s="6">
         <f t="shared" ref="A38:A41" si="6">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45148</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C38" s="1">
         <v>17.0</v>
@@ -888,14 +1350,26 @@
       <c r="D38" s="1">
         <v>257.0</v>
       </c>
+      <c r="E38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="5">
+      <c r="A39" s="6">
         <f t="shared" si="6"/>
         <v>45148</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C39" s="1">
         <v>101.0</v>
@@ -903,14 +1377,26 @@
       <c r="D39" s="1">
         <v>337.0</v>
       </c>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="5">
+      <c r="A40" s="6">
         <f t="shared" si="6"/>
         <v>45148</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C40" s="1">
         <v>8.0</v>
@@ -918,14 +1404,26 @@
       <c r="D40" s="1">
         <v>287.0</v>
       </c>
+      <c r="E40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="5">
+      <c r="A41" s="6">
         <f t="shared" si="6"/>
         <v>45148</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C41" s="1">
         <v>27.0</v>
@@ -933,14 +1431,26 @@
       <c r="D41" s="1">
         <v>240.0</v>
       </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="5">
+      <c r="A42" s="6">
         <f t="shared" ref="A42:A45" si="7">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45149</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C42" s="1">
         <v>24.0</v>
@@ -948,14 +1458,26 @@
       <c r="D42" s="1">
         <v>280.0</v>
       </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="5">
+      <c r="A43" s="6">
         <f t="shared" si="7"/>
         <v>45149</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C43" s="1">
         <v>75.0</v>
@@ -963,14 +1485,26 @@
       <c r="D43" s="1">
         <v>261.0</v>
       </c>
+      <c r="E43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="5">
+      <c r="A44" s="6">
         <f t="shared" si="7"/>
         <v>45149</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C44" s="1">
         <v>1.0</v>
@@ -978,14 +1512,26 @@
       <c r="D44" s="1">
         <v>123.0</v>
       </c>
+      <c r="E44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="5">
+      <c r="A45" s="6">
         <f t="shared" si="7"/>
         <v>45149</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C45" s="1">
         <v>24.0</v>
@@ -993,14 +1539,26 @@
       <c r="D45" s="1">
         <v>222.0</v>
       </c>
+      <c r="E45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="5">
+      <c r="A46" s="6">
         <f t="shared" ref="A46:A49" si="8">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45150</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C46" s="1">
         <v>10.0</v>
@@ -1008,14 +1566,26 @@
       <c r="D46" s="1">
         <v>140.0</v>
       </c>
+      <c r="E46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="5">
+      <c r="A47" s="6">
         <f t="shared" si="8"/>
         <v>45150</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1">
         <v>58.0</v>
@@ -1023,14 +1593,26 @@
       <c r="D47" s="1">
         <v>247.0</v>
       </c>
+      <c r="E47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="5">
+      <c r="A48" s="6">
         <f t="shared" si="8"/>
         <v>45150</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C48" s="1">
         <v>1.0</v>
@@ -1038,14 +1620,26 @@
       <c r="D48" s="1">
         <v>83.0</v>
       </c>
+      <c r="E48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="5">
+      <c r="A49" s="6">
         <f t="shared" si="8"/>
         <v>45150</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C49" s="1">
         <v>23.0</v>
@@ -1053,14 +1647,26 @@
       <c r="D49" s="1">
         <v>87.0</v>
       </c>
+      <c r="E49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="5">
+      <c r="A50" s="6">
         <f t="shared" ref="A50:A53" si="9">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45151</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C50" s="1">
         <v>9.0</v>
@@ -1068,14 +1674,26 @@
       <c r="D50" s="1">
         <v>137.0</v>
       </c>
+      <c r="E50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="5">
+      <c r="A51" s="6">
         <f t="shared" si="9"/>
         <v>45151</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C51" s="1">
         <v>35.0</v>
@@ -1083,14 +1701,26 @@
       <c r="D51" s="1">
         <v>172.0</v>
       </c>
+      <c r="E51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="5">
+      <c r="A52" s="6">
         <f t="shared" si="9"/>
         <v>45151</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C52" s="1">
         <v>3.0</v>
@@ -1098,14 +1728,26 @@
       <c r="D52" s="1">
         <v>123.0</v>
       </c>
+      <c r="E52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="5">
+      <c r="A53" s="6">
         <f t="shared" si="9"/>
         <v>45151</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C53" s="1">
         <v>75.0</v>
@@ -1113,14 +1755,26 @@
       <c r="D53" s="1">
         <v>285.0</v>
       </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="5">
+      <c r="A54" s="6">
         <f t="shared" ref="A54:A57" si="10">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45152</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C54" s="1">
         <v>20.0</v>
@@ -1128,14 +1782,26 @@
       <c r="D54" s="1">
         <v>185.0</v>
       </c>
+      <c r="E54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="5">
+      <c r="A55" s="6">
         <f t="shared" si="10"/>
         <v>45152</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C55" s="1">
         <v>157.0</v>
@@ -1143,14 +1809,26 @@
       <c r="D55" s="1">
         <v>346.0</v>
       </c>
+      <c r="E55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="5">
+      <c r="A56" s="6">
         <f t="shared" si="10"/>
         <v>45152</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C56" s="1">
         <v>8.0</v>
@@ -1158,14 +1836,26 @@
       <c r="D56" s="1">
         <v>143.0</v>
       </c>
+      <c r="E56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="5">
+      <c r="A57" s="6">
         <f t="shared" si="10"/>
         <v>45152</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C57" s="1">
         <v>24.0</v>
@@ -1173,14 +1863,26 @@
       <c r="D57" s="1">
         <v>269.0</v>
       </c>
+      <c r="E57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="5">
+      <c r="A58" s="6">
         <f t="shared" ref="A58:A61" si="11">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45153</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C58" s="1">
         <v>19.0</v>
@@ -1188,14 +1890,26 @@
       <c r="D58" s="1">
         <v>179.0</v>
       </c>
+      <c r="E58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="5">
+      <c r="A59" s="6">
         <f t="shared" si="11"/>
         <v>45153</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C59" s="1">
         <v>34.0</v>
@@ -1203,14 +1917,26 @@
       <c r="D59" s="1">
         <v>205.0</v>
       </c>
+      <c r="E59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="5">
+      <c r="A60" s="6">
         <f t="shared" si="11"/>
         <v>45153</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C60" s="1">
         <v>2.0</v>
@@ -1218,14 +1944,26 @@
       <c r="D60" s="1">
         <v>164.0</v>
       </c>
+      <c r="E60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="5">
+      <c r="A61" s="6">
         <f t="shared" si="11"/>
         <v>45153</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C61" s="1">
         <v>24.0</v>
@@ -1233,14 +1971,26 @@
       <c r="D61" s="1">
         <v>211.0</v>
       </c>
+      <c r="E61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="5">
+      <c r="A62" s="6">
         <f t="shared" ref="A62:A65" si="12">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45154</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C62" s="1">
         <v>15.0</v>
@@ -1248,14 +1998,26 @@
       <c r="D62" s="1">
         <v>262.0</v>
       </c>
+      <c r="E62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="5">
+      <c r="A63" s="6">
         <f t="shared" si="12"/>
         <v>45154</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C63" s="1">
         <v>120.0</v>
@@ -1263,14 +2025,26 @@
       <c r="D63" s="1">
         <v>357.0</v>
       </c>
+      <c r="E63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="5">
+      <c r="A64" s="6">
         <f t="shared" si="12"/>
         <v>45154</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C64" s="1">
         <v>5.0</v>
@@ -1278,14 +2052,26 @@
       <c r="D64" s="1">
         <v>153.0</v>
       </c>
+      <c r="E64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="5">
+      <c r="A65" s="6">
         <f t="shared" si="12"/>
         <v>45154</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C65" s="1">
         <v>46.0</v>
@@ -1293,545 +2079,1628 @@
       <c r="D65" s="1">
         <v>412.0</v>
       </c>
+      <c r="E65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="5">
+      <c r="A66" s="6">
         <f t="shared" ref="A66:A69" si="13">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45155</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C66" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="D66" s="1">
+        <v>290.0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="5">
+      <c r="A67" s="6">
         <f t="shared" si="13"/>
         <v>45155</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C67" s="1">
+        <v>94.0</v>
+      </c>
+      <c r="D67" s="1">
+        <v>348.0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="5">
+      <c r="A68" s="6">
         <f t="shared" si="13"/>
         <v>45155</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C68" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>305.0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="5">
+      <c r="A69" s="6">
         <f t="shared" si="13"/>
         <v>45155</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C69" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>285.0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="5">
+      <c r="A70" s="6">
         <f t="shared" ref="A70:A73" si="14">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45156</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C70" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="D70" s="1">
+        <v>311.0</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="5">
+      <c r="A71" s="6">
         <f t="shared" si="14"/>
         <v>45156</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C71" s="1">
+        <v>76.0</v>
+      </c>
+      <c r="D71" s="1">
+        <v>260.0</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="5">
+      <c r="A72" s="6">
         <f t="shared" si="14"/>
         <v>45156</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D72" s="1">
+        <v>113.0</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="5">
+      <c r="A73" s="6">
         <f t="shared" si="14"/>
         <v>45156</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C73" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="D73" s="1">
+        <v>292.0</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="5">
+      <c r="A74" s="6">
         <f t="shared" ref="A74:A77" si="15">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45157</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C74" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="D74" s="1">
+        <v>160.0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="5">
+      <c r="A75" s="6">
         <f t="shared" si="15"/>
         <v>45157</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C75" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D75" s="1">
+        <v>291.0</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G75" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="5">
+      <c r="A76" s="6">
         <f t="shared" si="15"/>
         <v>45157</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>111.0</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G76" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="5">
+      <c r="A77" s="6">
         <f t="shared" si="15"/>
         <v>45157</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C77" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>126.0</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="5">
+      <c r="A78" s="6">
         <f t="shared" ref="A78:A81" si="16">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45158</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C78" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="D78" s="1">
+        <v>151.0</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="5">
+      <c r="A79" s="6">
         <f t="shared" si="16"/>
         <v>45158</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C79" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="D79" s="1">
+        <v>182.0</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="5">
+      <c r="A80" s="6">
         <f t="shared" si="16"/>
         <v>45158</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>167.0</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="5">
+      <c r="A81" s="6">
         <f t="shared" si="16"/>
         <v>45158</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C81" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="5">
+      <c r="A82" s="6">
         <f t="shared" ref="A82:A85" si="17">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45159</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C82" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="5">
+      <c r="A83" s="6">
         <f t="shared" si="17"/>
         <v>45159</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C83" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="D83" s="1">
+        <v>360.0</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="5">
+      <c r="A84" s="6">
         <f t="shared" si="17"/>
         <v>45159</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C84" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>224.0</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="5">
+      <c r="A85" s="6">
         <f t="shared" si="17"/>
         <v>45159</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C85" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="D85" s="1">
+        <v>356.0</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="5">
+      <c r="A86" s="6">
         <f t="shared" ref="A86:A89" si="18">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45160</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C86" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="D86" s="1">
+        <v>251.0</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="5">
+      <c r="A87" s="6">
         <f t="shared" si="18"/>
         <v>45160</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C87" s="1">
+        <v>108.0</v>
+      </c>
+      <c r="D87" s="1">
+        <v>390.0</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="5">
+      <c r="A88" s="6">
         <f t="shared" si="18"/>
         <v>45160</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C88" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D88" s="1">
+        <v>265.0</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="5">
+      <c r="A89" s="6">
         <f t="shared" si="18"/>
         <v>45160</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C89" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="D89" s="1">
+        <v>235.0</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G89" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="5">
+      <c r="A90" s="6">
         <f t="shared" ref="A90:A93" si="19">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45161</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C90" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="D90" s="1">
+        <v>233.0</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G90" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="5">
+      <c r="A91" s="6">
         <f t="shared" si="19"/>
         <v>45161</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C91" s="1">
+        <v>119.0</v>
+      </c>
+      <c r="D91" s="1">
+        <v>373.0</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G91" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="5">
+      <c r="A92" s="6">
         <f t="shared" si="19"/>
         <v>45161</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C92" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D92" s="1">
+        <v>135.0</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G92" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="5">
+      <c r="A93" s="6">
         <f t="shared" si="19"/>
         <v>45161</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C93" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="D93" s="1">
+        <v>443.0</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G93" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H93" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="5">
+      <c r="A94" s="6">
         <f t="shared" ref="A94:A97" si="20">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45162</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C94" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="D94" s="1">
+        <v>257.0</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G94" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="5">
+      <c r="A95" s="6">
         <f t="shared" si="20"/>
         <v>45162</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C95" s="1">
+        <v>110.0</v>
+      </c>
+      <c r="D95" s="1">
+        <v>318.0</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G95" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="5">
+      <c r="A96" s="6">
         <f t="shared" si="20"/>
         <v>45162</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C96" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="D96" s="1">
+        <v>288.0</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G96" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="5">
+      <c r="A97" s="6">
         <f t="shared" si="20"/>
         <v>45162</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C97" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="D97" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G97" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H97" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="5">
+      <c r="A98" s="6">
         <f t="shared" ref="A98:A101" si="21">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45163</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C98" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="D98" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G98" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H98" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="5">
+      <c r="A99" s="6">
         <f t="shared" si="21"/>
         <v>45163</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C99" s="1">
+        <v>67.0</v>
+      </c>
+      <c r="D99" s="1">
+        <v>164.0</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G99" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H99" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="5">
+      <c r="A100" s="6">
         <f t="shared" si="21"/>
         <v>45163</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D100" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G100" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H100" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="5">
+      <c r="A101" s="6">
         <f t="shared" si="21"/>
         <v>45163</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C101" s="1">
+        <v>42.0</v>
+      </c>
+      <c r="D101" s="1">
+        <v>229.0</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G101" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H101" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="5">
+      <c r="A102" s="6">
         <f t="shared" ref="A102:A105" si="22">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45164</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C102" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="D102" s="1">
+        <v>150.0</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G102" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="5">
+      <c r="A103" s="6">
         <f t="shared" si="22"/>
         <v>45164</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C103" s="1">
+        <v>86.0</v>
+      </c>
+      <c r="D103" s="1">
+        <v>305.0</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G103" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="5">
+      <c r="A104" s="6">
         <f t="shared" si="22"/>
         <v>45164</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C104" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D104" s="1">
+        <v>104.0</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G104" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H104" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="5">
+      <c r="A105" s="6">
         <f t="shared" si="22"/>
         <v>45164</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C105" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="D105" s="1">
+        <v>92.0</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G105" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H105" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="5">
+      <c r="A106" s="6">
         <f t="shared" ref="A106:A109" si="23">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45165</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C106" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="D106" s="1">
+        <v>157.0</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G106" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="5">
+      <c r="A107" s="6">
         <f t="shared" si="23"/>
         <v>45165</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C107" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="D107" s="1">
+        <v>193.0</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G107" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H107" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="5">
+      <c r="A108" s="6">
         <f t="shared" si="23"/>
         <v>45165</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C108" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G108" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H108" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="5">
+      <c r="A109" s="6">
         <f t="shared" si="23"/>
         <v>45165</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C109" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D109" s="1">
+        <v>270.0</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G109" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H109" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="5">
+      <c r="A110" s="6">
         <f t="shared" ref="A110:A113" si="24">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45166</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C110" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="D110" s="1">
+        <v>194.0</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="5">
+      <c r="A111" s="6">
         <f t="shared" si="24"/>
         <v>45166</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C111" s="1">
+        <v>101.0</v>
+      </c>
+      <c r="D111" s="1">
+        <v>296.0</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G111" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H111" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="5">
+      <c r="A112" s="6">
         <f t="shared" si="24"/>
         <v>45166</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C112" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="D112" s="1">
+        <v>177.0</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G112" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="5">
+      <c r="A113" s="6">
         <f t="shared" si="24"/>
         <v>45166</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C113" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="D113" s="1">
+        <v>314.0</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G113" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="5">
+      <c r="A114" s="6">
         <f t="shared" ref="A114:A117" si="25">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45167</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C114" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="D114" s="1">
+        <v>230.0</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H114" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="5">
+      <c r="A115" s="6">
         <f t="shared" si="25"/>
         <v>45167</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C115" s="1">
+        <v>109.0</v>
+      </c>
+      <c r="D115" s="1">
+        <v>307.0</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G115" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H115" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="5">
+      <c r="A116" s="6">
         <f t="shared" si="25"/>
         <v>45167</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C116" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D116" s="1">
+        <v>174.0</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G116" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H116" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="5">
+      <c r="A117" s="6">
         <f t="shared" si="25"/>
         <v>45167</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C117" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="D117" s="1">
+        <v>140.0</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F117" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G117" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H117" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="5">
+      <c r="A118" s="6">
         <f t="shared" ref="A118:A121" si="26">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45168</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C118" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="D118" s="1">
+        <v>126.0</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F118" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G118" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H118" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="5">
+      <c r="A119" s="6">
         <f t="shared" si="26"/>
         <v>45168</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C119" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="D119" s="1">
+        <v>152.0</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G119" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H119" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="5">
+      <c r="A120" s="6">
         <f t="shared" si="26"/>
         <v>45168</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C120" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D120" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G120" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H120" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="5">
+      <c r="A121" s="6">
         <f t="shared" si="26"/>
         <v>45168</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C121" s="1">
+        <v>44.0</v>
+      </c>
+      <c r="D121" s="1">
+        <v>209.0</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F121" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G121" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H121" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="5">
+      <c r="A122" s="6">
         <f t="shared" ref="A122:A125" si="27">A2 + (INT((ROW()-ROW($B$2))/4))</f>
         <v>45169</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C122" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="D122" s="1">
+        <v>180.0</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F122" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G122" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H122" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="5">
+      <c r="A123" s="6">
         <f t="shared" si="27"/>
         <v>45169</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C123" s="1">
+        <v>126.0</v>
+      </c>
+      <c r="D123" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F123" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G123" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H123" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="5">
+      <c r="A124" s="6">
         <f t="shared" si="27"/>
         <v>45169</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C124" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="D124" s="1">
+        <v>252.0</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G124" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H124" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="5">
+      <c r="A125" s="6">
         <f t="shared" si="27"/>
         <v>45169</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C125" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="D125" s="1">
+        <v>191.0</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F125" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G125" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H125" s="1">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>